<commit_message>
Updated data inputs and fixed bugs.
</commit_message>
<xml_diff>
--- a/Data/Asthma/Transition probabilities/transition data_weekly_recalibrate2.xlsx
+++ b/Data/Asthma/Transition probabilities/transition data_weekly_recalibrate2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaya\Box\AA_Sigal_Documents\Climate - Health\Wildfire Asthma Microsim\Modeling\Data\Asthma\Transition probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF233ED0-C731-4922-BE10-60FF46AAEEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400FC5DA-D9C7-4E13-A535-5598D57B58C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" tabRatio="697" xr2:uid="{9B6F3090-D219-4CD1-9FEE-A2B042DB449C}"/>
+    <workbookView xWindow="37830" yWindow="-930" windowWidth="17415" windowHeight="11595" tabRatio="697" xr2:uid="{9B6F3090-D219-4CD1-9FEE-A2B042DB449C}"/>
   </bookViews>
   <sheets>
     <sheet name="transition_prob" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="61">
   <si>
     <t>Value by definition</t>
   </si>
@@ -238,17 +238,90 @@
   <si>
     <t>Below from Lemmetyinen et al 2018 (Finland)</t>
   </si>
+  <si>
+    <t>pmean = pref*propref + pref*prop1*rr1 + pref*prop2*rr2</t>
+  </si>
+  <si>
+    <t>pmean = pref * (propref + prop1*rr1 + prop2*rr2)</t>
+  </si>
+  <si>
+    <t>prop none to mild sx</t>
+  </si>
+  <si>
+    <t>prop moderate sx</t>
+  </si>
+  <si>
+    <t>prop severe sx</t>
+  </si>
+  <si>
+    <t>prob none-mild sx</t>
+  </si>
+  <si>
+    <t>rate yr none-mild</t>
+  </si>
+  <si>
+    <t>rate yr moderate</t>
+  </si>
+  <si>
+    <t>rate yr severe</t>
+  </si>
+  <si>
+    <t>rate wk none-mild</t>
+  </si>
+  <si>
+    <t>rate wk moderate</t>
+  </si>
+  <si>
+    <t>rate wk severe</t>
+  </si>
+  <si>
+    <t>rate 10wk moderate</t>
+  </si>
+  <si>
+    <t>rate 10wk severe</t>
+  </si>
+  <si>
+    <t>rate 10wk none-mild</t>
+  </si>
+  <si>
+    <t>prob (annual)=</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>prob 10wk none to mild</t>
+  </si>
+  <si>
+    <t>prob 10wk moderate</t>
+  </si>
+  <si>
+    <t>prob 10wk severe</t>
+  </si>
+  <si>
+    <t>prob wk none to mild</t>
+  </si>
+  <si>
+    <t>prob wk moderate</t>
+  </si>
+  <si>
+    <t>prob wk severe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="7">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.000000000"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.000000000_);_(* \(#,##0.000000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +366,13 @@
     <font>
       <sz val="11"/>
       <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -371,10 +451,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -448,8 +529,12 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1240,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFE29CD-D7CE-45DF-83DF-7AAE57E0BCAE}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1351,11 +1436,11 @@
         <v>0</v>
       </c>
       <c r="I3" s="20">
-        <v>0</v>
+        <v>1.6063380248820813E-4</v>
       </c>
       <c r="J3" s="25">
         <f t="shared" ref="J3:J7" si="0">1-SUM(B3:I3)</f>
-        <v>0.69130000000000003</v>
+        <v>0.69113936619751182</v>
       </c>
       <c r="K3" s="34"/>
       <c r="M3" s="8" t="s">
@@ -1388,11 +1473,11 @@
         <v>0</v>
       </c>
       <c r="I4" s="20">
-        <v>0</v>
+        <v>1.6063380248820813E-4</v>
       </c>
       <c r="J4" s="25">
         <f t="shared" si="0"/>
-        <v>0.81308000000000002</v>
+        <v>0.81291936619751182</v>
       </c>
       <c r="K4" s="16"/>
       <c r="M4" s="9" t="s">
@@ -1425,11 +1510,11 @@
         <v>0</v>
       </c>
       <c r="I5" s="20">
-        <v>0</v>
+        <v>2.5860775107100498E-4</v>
       </c>
       <c r="J5" s="25">
         <f t="shared" si="0"/>
-        <v>0.75570999999999999</v>
+        <v>0.75545139224892899</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>0</v>
@@ -1461,11 +1546,11 @@
         <v>2.3076896449314432E-6</v>
       </c>
       <c r="I6" s="20">
-        <v>0</v>
+        <v>2.5860775107100498E-4</v>
       </c>
       <c r="J6" s="25">
         <f t="shared" si="0"/>
-        <v>0.6751476923103551</v>
+        <v>0.67488908455928409</v>
       </c>
       <c r="K6" s="27"/>
       <c r="M6" s="31" t="s">
@@ -1498,11 +1583,11 @@
         <v>2.3076896449314432E-6</v>
       </c>
       <c r="I7" s="20">
-        <v>0</v>
+        <v>5.1233170374809234E-4</v>
       </c>
       <c r="J7" s="25">
         <f t="shared" si="0"/>
-        <v>0.63602769231035505</v>
+        <v>0.63551536060660696</v>
       </c>
       <c r="K7" s="16"/>
       <c r="M7" s="32" t="s">
@@ -1569,33 +1654,44 @@
       </c>
       <c r="J9" s="16"/>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K11">
+        <v>1.6063380248820813E-4</v>
+      </c>
+    </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>7</v>
       </c>
+      <c r="K12">
+        <v>2.5860775107100498E-4</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <v>5.1233170374809234E-4</v>
+      </c>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M14" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D25" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="30"/>
       <c r="B26" s="20">
         <v>0</v>
@@ -1604,7 +1700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="28"/>
       <c r="B27" s="20">
         <v>2.5999999999999998E-4</v>
@@ -1617,111 +1713,315 @@
         <v>1.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="26"/>
       <c r="B28" s="20">
         <v>2.5999999999999998E-4</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E28">
-        <f>1-EXP(-E27/52)</f>
-        <v>2.6150426333648724E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <f>1-EXP(-E27)</f>
+        <v>1.3507937821110039E-2</v>
+      </c>
+      <c r="K28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="21"/>
       <c r="B29" s="20">
         <v>3.8879575775713215E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29">
+        <f>1-EXP(-E27/52)</f>
+        <v>2.6150426333648724E-4</v>
+      </c>
+      <c r="K29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="18"/>
       <c r="B30" s="20">
         <v>3.8879575775713215E-4</v>
       </c>
-      <c r="D30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="21"/>
       <c r="B31" s="20">
         <v>7.7759151551426431E-4</v>
       </c>
       <c r="D31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
         <v>27</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <f>0.12/1000</f>
         <v>1.1999999999999999E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D32" t="s">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33">
+        <f>1-EXP(-E32)</f>
+        <v>1.1999280028796022E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
         <v>30</v>
       </c>
-      <c r="E32">
-        <f>1-EXP(-E31/52)</f>
+      <c r="E34">
+        <f>1-EXP(-E32/52)</f>
         <v>2.3076896449314432E-6</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D34" t="s">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D35" t="s">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
         <v>27</v>
       </c>
-      <c r="E35">
-        <f>E27-E31</f>
+      <c r="E37">
+        <f>E27-E32</f>
         <v>1.3479999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D36" t="s">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38">
+        <f>1-EXP(-E37)</f>
+        <v>1.3389551670621502E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D39" t="s">
         <v>30</v>
       </c>
-      <c r="E36">
-        <f>1-EXP(-E35/52)</f>
+      <c r="E39">
+        <f>1-EXP(-E37/52)</f>
         <v>2.591971718380881E-4</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D38" t="s">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D41" t="s">
         <v>34</v>
       </c>
-      <c r="E38">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D39" t="s">
+      <c r="E41">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D42" t="s">
         <v>33</v>
       </c>
-      <c r="E39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D41" t="s">
+      <c r="E42">
+        <v>3.19</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44">
+        <v>0.64700000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="39">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47">
+        <f>E38 / (E43 + E44*E41 + E45*E42)</f>
+        <v>8.2975773675048204E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D48" t="s">
         <v>35</v>
       </c>
-      <c r="E41">
-        <f>E36*E38</f>
-        <v>3.8879575775713215E-4</v>
-      </c>
-    </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D42" t="s">
+      <c r="E48" s="40">
+        <f>E47*E41</f>
+        <v>1.3359099561682762E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D49" t="s">
         <v>36</v>
       </c>
-      <c r="E42">
-        <f>E36*E39</f>
-        <v>7.7759151551426431E-4</v>
+      <c r="E49">
+        <f>E47*E42</f>
+        <v>2.6469271802340377E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51">
+        <f>E37 / (E43 + E44*E41 +E45*E42)</f>
+        <v>8.3536286849231877E-3</v>
+      </c>
+      <c r="F51" s="41">
+        <f>-LN(1-E47)</f>
+        <v>8.3321938844046692E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D52" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52">
+        <f>E51*E41</f>
+        <v>1.3449342182726334E-2</v>
+      </c>
+      <c r="F52" s="41">
+        <f t="shared" ref="F52:F53" si="1">-LN(1-E48)</f>
+        <v>1.3449135093752562E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D53" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53">
+        <f>E51*E42</f>
+        <v>2.6648075504904969E-2</v>
+      </c>
+      <c r="F53" s="41">
+        <f t="shared" si="1"/>
+        <v>2.6825890006855195E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D55" t="s">
+        <v>47</v>
+      </c>
+      <c r="E55">
+        <f>E51/52</f>
+        <v>1.6064670547929208E-4</v>
+      </c>
+      <c r="G55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H55">
+        <f>E55*10</f>
+        <v>1.6064670547929209E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
+        <v>48</v>
+      </c>
+      <c r="E56">
+        <f t="shared" ref="E56:E57" si="2">E52/52</f>
+        <v>2.5864119582166026E-4</v>
+      </c>
+      <c r="G56" t="s">
+        <v>50</v>
+      </c>
+      <c r="H56">
+        <f t="shared" ref="H56:H57" si="3">E56*10</f>
+        <v>2.5864119582166027E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>5.1246299047894169E-4</v>
+      </c>
+      <c r="G57" t="s">
+        <v>51</v>
+      </c>
+      <c r="H57" s="40">
+        <f t="shared" si="3"/>
+        <v>5.1246299047894173E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D59" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59">
+        <f>1-EXP(-E55)</f>
+        <v>1.6063380248820813E-4</v>
+      </c>
+      <c r="G59" t="s">
+        <v>55</v>
+      </c>
+      <c r="H59">
+        <f>1-EXP(-H55)</f>
+        <v>1.6051773772944866E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D60" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60">
+        <f t="shared" ref="E60:E61" si="4">1-EXP(-E56)</f>
+        <v>2.5860775107100498E-4</v>
+      </c>
+      <c r="G60" t="s">
+        <v>56</v>
+      </c>
+      <c r="H60" s="40">
+        <f t="shared" ref="H60:H61" si="5">1-EXP(-H56)</f>
+        <v>2.5830700765895331E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D61" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="4"/>
+        <v>5.1233170374809234E-4</v>
+      </c>
+      <c r="G61" t="s">
+        <v>57</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="5"/>
+        <v>5.1115213906127721E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2626,7 +2926,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2687,7 +2987,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="15">
-        <v>18.77</v>
+        <v>1</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>1</v>
@@ -2719,7 +3019,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="15">
-        <v>18.77</v>
+        <v>1</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>2</v>
@@ -2751,7 +3051,7 @@
         <v>7.24</v>
       </c>
       <c r="I4" s="15">
-        <v>18.77</v>
+        <v>1</v>
       </c>
       <c r="M4" s="9" t="s">
         <v>3</v>
@@ -2783,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="15">
-        <v>18.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -2812,7 +3112,7 @@
         <v>7.75</v>
       </c>
       <c r="I6" s="15">
-        <v>18.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -2841,7 +3141,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="15">
-        <v>18.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>